<commit_message>
check of threshold values
</commit_message>
<xml_diff>
--- a/klassegr/klassegrenser_NSI.xlsx
+++ b/klassegr/klassegrenser_NSI.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\61308-01_fu_intern_hanno_sandvik\NI_vannf\klassegr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EB9E87-9B27-4F1B-AE93-7D7B8C6F3F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817CD726-3834-451E-ABCF-63C3B5B16E9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3A75F986-4B69-4A9F-BCAA-E28782105059}"/>
   </bookViews>
@@ -504,7 +504,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,7 +729,7 @@
         <v>14</v>
       </c>
       <c r="F8">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="G8">
         <v>24</v>
@@ -758,7 +758,7 @@
         <v>14</v>
       </c>
       <c r="F9">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="G9">
         <v>24</v>
@@ -787,7 +787,7 @@
         <v>14</v>
       </c>
       <c r="F10">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="G10">
         <v>24</v>
@@ -874,7 +874,7 @@
         <v>14</v>
       </c>
       <c r="F13">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="G13">
         <v>24</v>
@@ -903,7 +903,7 @@
         <v>14</v>
       </c>
       <c r="F14">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="G14">
         <v>24</v>
@@ -932,7 +932,7 @@
         <v>14</v>
       </c>
       <c r="F15">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="G15">
         <v>24</v>

</xml_diff>